<commit_message>
minor changes to tables
</commit_message>
<xml_diff>
--- a/ms/3. nature ecology & evolution/1. initial submission natecoevol201012000T /Supplementary_model tables_S1-S8.xlsx
+++ b/ms/3. nature ecology & evolution/1. initial submission natecoevol201012000T /Supplementary_model tables_S1-S8.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_diff_meta/ms/nature communications ms/Supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_diff_meta/ms/3. nature ecology &amp; evolution/1. initial submission natecoevol201012000T /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF626EE-F44B-CF41-9BC8-B1B77C8025FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8AE579-5A63-6B4F-AAC1-D1579E4EB8FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" firstSheet="1" activeTab="8" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="7" r:id="rId1"/>
@@ -1364,21 +1364,6 @@
     <t>-0.77, 0.76</t>
   </si>
   <si>
-    <t>S5 - Contrast models for each of the five taxonomic groups with personality trait and SSD as moderators. Activity</t>
-  </si>
-  <si>
-    <t>S7 - Contrast models for each of the five taxonomic groups with personality trait and SSD as moderators. Boldness</t>
-  </si>
-  <si>
-    <t>S6 - Contrast models for each of the five taxonomic groups with personality trait and SSD as moderators. Aggression</t>
-  </si>
-  <si>
-    <t>S8 - Contrast models for each of the five taxonomic groups with personality trait and SSD as moderators. Exploration</t>
-  </si>
-  <si>
-    <t>S5: Contrast models - Activity (intercept) and SSD - only have enough data for inverts and mammals</t>
-  </si>
-  <si>
     <t>-0.15, 0.25</t>
   </si>
   <si>
@@ -1400,15 +1385,6 @@
     <t>-1.74, 2.62</t>
   </si>
   <si>
-    <t>S6: Contrast models - Aggression (intercept) and SSD - only have enough data for fish and mammals</t>
-  </si>
-  <si>
-    <t>S7: Contrast models - Boldness (intercept) and SSD - only have enough data for birds, fish, inverts and mammals</t>
-  </si>
-  <si>
-    <t>S8: Contrast models - Exploration (intercept) and SSD - only have enough data for mammals</t>
-  </si>
-  <si>
     <t>-0.03, 0.16</t>
   </si>
   <si>
@@ -1620,6 +1596,30 @@
   </si>
   <si>
     <t>-0.54, 1.10</t>
+  </si>
+  <si>
+    <t>S5 - Subset models for each of the five taxonomic groups with personality trait and SSD as moderators. Activity</t>
+  </si>
+  <si>
+    <t>S6 - Subset models for each of the five taxonomic groups with personality trait and SSD as moderators. Aggression</t>
+  </si>
+  <si>
+    <t>S7 - Subset models for each of the five taxonomic groups with personality trait and SSD as moderators. Boldness</t>
+  </si>
+  <si>
+    <t>S8 - Subset models for each of the five taxonomic groups with personality trait and SSD as moderators. Exploration</t>
+  </si>
+  <si>
+    <t>S5: Subset models - Activity (intercept) and SSD - only have enough data for inverts and mammals</t>
+  </si>
+  <si>
+    <t>S6: Subset models - Aggression (intercept) and SSD - only have enough data for fish and mammals</t>
+  </si>
+  <si>
+    <t>S7: Subset models - Boldness (intercept) and SSD - only have enough data for birds, fish, inverts and mammals</t>
+  </si>
+  <si>
+    <t>S8: Subset models - Exploration (intercept) and SSD - only have enough data for mammals</t>
   </si>
 </sst>
 </file>
@@ -2108,15 +2108,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C130962E-6B74-C444-8BBE-259CB0E6BD42}">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -2146,22 +2146,22 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>443</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>445</v>
+        <v>522</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>444</v>
+        <v>523</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>446</v>
+        <v>524</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
@@ -2233,7 +2233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAF7C5E-35C2-0343-8AC1-0E9A3B22FC74}">
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -4043,7 +4043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF86D62B-22BF-1846-B677-968C777627E8}">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView topLeftCell="N2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
@@ -7640,13 +7640,13 @@
         <v>0.16</v>
       </c>
       <c r="W16" s="24" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="X16" s="5">
         <v>0.76</v>
       </c>
       <c r="Y16" s="24" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="Z16" s="5">
         <v>0.45</v>
@@ -7777,13 +7777,13 @@
         <v>0.52</v>
       </c>
       <c r="W17" s="24" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="X17" s="5">
         <v>1.01</v>
       </c>
       <c r="Y17" s="24" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="Z17" s="5">
         <v>0.32</v>
@@ -7915,13 +7915,13 @@
         <v>0.31</v>
       </c>
       <c r="W18" s="24" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="X18" s="5">
         <v>1.47</v>
       </c>
       <c r="Y18" s="36" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="Z18" s="5">
         <v>0.14000000000000001</v>
@@ -8052,13 +8052,13 @@
         <v>-0.15</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="X19" s="5">
         <v>-0.42</v>
       </c>
       <c r="Y19" s="24" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="Z19" s="5">
         <v>0.68</v>
@@ -8189,13 +8189,13 @@
         <v>0.23</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="X20" s="5">
         <v>0.56999999999999995</v>
       </c>
       <c r="Y20" s="24" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="Z20" s="5">
         <v>0.56999999999999995</v>
@@ -8323,7 +8323,7 @@
         <v>-0.87</v>
       </c>
       <c r="W21" s="29" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="X21" s="22">
         <v>-1.23</v>
@@ -8460,13 +8460,13 @@
         <v>1.31</v>
       </c>
       <c r="W22" s="36" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="X22" s="13">
         <v>0.62</v>
       </c>
       <c r="Y22" s="36" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="Z22" s="13">
         <v>0.53</v>
@@ -8601,13 +8601,13 @@
         <v>1.05</v>
       </c>
       <c r="W23" s="36" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="X23" s="13">
         <v>1.52</v>
       </c>
       <c r="Y23" s="36" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="Z23" s="13">
         <v>0.13</v>
@@ -8742,13 +8742,13 @@
         <v>0.21</v>
       </c>
       <c r="W24" s="36" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="X24" s="13">
         <v>0.14000000000000001</v>
       </c>
       <c r="Y24" s="36" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="Z24" s="13">
         <v>0.89</v>
@@ -9056,7 +9056,7 @@
         <v>0.8</v>
       </c>
       <c r="W28" s="5" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="X28" s="5" t="s">
         <v>39</v>
@@ -9668,13 +9668,13 @@
         <v>-0.03</v>
       </c>
       <c r="W36" s="31" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="X36" s="21">
         <v>-0.35</v>
       </c>
       <c r="Y36" s="31" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="Z36" s="21">
         <v>0.73</v>
@@ -9813,7 +9813,7 @@
         <v>0.15</v>
       </c>
       <c r="Y37" s="29" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="Z37" s="22">
         <v>0.88</v>
@@ -9944,13 +9944,13 @@
         <v>-0.03</v>
       </c>
       <c r="W38" s="29" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="X38" s="22">
         <v>-0.37</v>
       </c>
       <c r="Y38" s="36" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="Z38" s="22">
         <v>0.71</v>
@@ -10082,13 +10082,13 @@
         <v>0.04</v>
       </c>
       <c r="W39" s="29" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="X39" s="22">
         <v>0.23</v>
       </c>
       <c r="Y39" s="36" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="Z39" s="22">
         <v>0.81</v>
@@ -10219,13 +10219,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="W40" s="29" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="X40" s="22">
         <v>1.32</v>
       </c>
       <c r="Y40" s="36" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="Z40" s="22">
         <v>0.19</v>
@@ -10353,7 +10353,7 @@
         <v>0.17</v>
       </c>
       <c r="W41" s="29" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="X41" s="22">
         <v>0.55000000000000004</v>
@@ -10489,13 +10489,13 @@
         <v>0.67</v>
       </c>
       <c r="W42" s="36" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="X42" s="13">
         <v>1.03</v>
       </c>
       <c r="Y42" s="36" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="Z42" s="13">
         <v>0.3</v>
@@ -10630,13 +10630,13 @@
         <v>-0.08</v>
       </c>
       <c r="W43" s="36" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="X43" s="13">
         <v>-0.2</v>
       </c>
       <c r="Y43" s="36" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="Z43" s="13">
         <v>0.84</v>
@@ -10771,13 +10771,13 @@
         <v>-0.34</v>
       </c>
       <c r="W44" s="36" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="X44" s="13">
         <v>-0.39</v>
       </c>
       <c r="Y44" s="36" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="Z44" s="13">
         <v>0.7</v>
@@ -11891,7 +11891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E1601E-514F-6C4E-8014-9481A0BF4F36}">
   <dimension ref="A1:AW97"/>
   <sheetViews>
-    <sheetView topLeftCell="K2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -16190,14 +16190,14 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>447</v>
+        <v>525</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -16234,7 +16234,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B5">
         <v>1069.5</v>
@@ -16243,7 +16243,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H5">
         <v>321.39999999999998</v>
@@ -16254,16 +16254,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B6">
         <v>0.67</v>
       </c>
       <c r="C6" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H6" s="4">
         <v>5.46</v>
@@ -16450,7 +16450,7 @@
         <v>0.31</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="D14" s="21">
         <v>0.83</v>
@@ -16466,7 +16466,7 @@
         <v>0.44</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="J14" s="21">
         <v>0.4</v>
@@ -16484,7 +16484,7 @@
         <v>-0.66</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D15" s="16">
         <v>-0.82</v>
@@ -16502,7 +16502,7 @@
         <v>-2.16</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="J15" s="14">
         <v>-2.34</v>
@@ -16524,7 +16524,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B17">
         <v>475.98</v>
@@ -16533,7 +16533,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H17">
         <v>146.26</v>
@@ -16544,22 +16544,22 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B18">
         <v>0.45</v>
       </c>
       <c r="C18" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H18">
         <v>0.13</v>
       </c>
       <c r="I18" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -16740,7 +16740,7 @@
         <v>-0.04</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="D26" s="21">
         <v>-0.36</v>
@@ -16756,7 +16756,7 @@
         <v>0.05</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="J26" s="21">
         <v>0.52</v>
@@ -16774,7 +16774,7 @@
         <v>0.27</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="D27" s="16">
         <v>0.67</v>
@@ -16792,7 +16792,7 @@
         <v>0.13</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="J27" s="16">
         <v>0.36</v>
@@ -16814,14 +16814,14 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>455</v>
+        <v>526</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -16858,7 +16858,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B5">
         <v>334.17</v>
@@ -16867,7 +16867,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H5">
         <v>313.77999999999997</v>
@@ -16878,22 +16878,22 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B6">
         <v>0.23</v>
       </c>
       <c r="C6" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H6" s="4">
         <v>3.92</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -17074,7 +17074,7 @@
         <v>-0.16</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="D14" s="21">
         <v>-0.41</v>
@@ -17090,7 +17090,7 @@
         <v>-0.09</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="J14" s="21">
         <v>-0.16</v>
@@ -17108,7 +17108,7 @@
         <v>0.27</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="D15" s="16">
         <v>0.48</v>
@@ -17126,7 +17126,7 @@
         <v>1.36</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="J15" s="14">
         <v>1.98</v>
@@ -17148,16 +17148,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B17">
         <v>68.27</v>
       </c>
       <c r="C17" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H17">
         <v>201.5</v>
@@ -17168,7 +17168,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B18">
         <v>0.15</v>
@@ -17177,7 +17177,7 @@
         <v>241</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H18">
         <v>0.01</v>
@@ -17364,7 +17364,7 @@
         <v>-0.12</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="D26" s="47">
         <v>-1.95</v>
@@ -17382,7 +17382,7 @@
         <v>0.09</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="J26" s="21">
         <v>0.59</v>
@@ -17400,7 +17400,7 @@
         <v>-0.13</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="D27" s="16">
         <v>-0.39</v>
@@ -17418,7 +17418,7 @@
         <v>-0.05</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="J27" s="16">
         <v>-7.0000000000000007E-2</v>
@@ -17439,15 +17439,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6C0B71-6C7E-C94B-9EF8-31E2F1C25E26}">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:24" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>456</v>
+        <v>527</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -17506,7 +17506,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B5">
         <v>1592.83</v>
@@ -17515,7 +17515,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H5">
         <v>614.58000000000004</v>
@@ -17524,7 +17524,7 @@
         <v>7</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="N5">
         <v>923.09</v>
@@ -17533,7 +17533,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="T5">
         <v>402.76</v>
@@ -17544,7 +17544,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B6">
         <v>0.15</v>
@@ -17553,25 +17553,25 @@
         <v>241</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H6" s="5">
         <v>1.07</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="N6">
         <v>0.46</v>
       </c>
       <c r="O6" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="T6" s="5">
         <v>0.92</v>
@@ -17930,7 +17930,7 @@
         <v>0.06</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="J14" s="21">
         <v>0.39</v>
@@ -17946,7 +17946,7 @@
         <v>0.18</v>
       </c>
       <c r="O14" s="28" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="P14" s="21">
         <v>1.68</v>
@@ -17962,7 +17962,7 @@
         <v>0.09</v>
       </c>
       <c r="U14" s="28" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="V14" s="21">
         <v>0.96</v>
@@ -17998,7 +17998,7 @@
         <v>-0.32</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="J15" s="16">
         <v>-1.03</v>
@@ -18016,7 +18016,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="P15" s="16">
         <v>0.68</v>
@@ -18034,7 +18034,7 @@
         <v>-0.16</v>
       </c>
       <c r="U15" s="27" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="V15" s="16">
         <v>-0.96</v>
@@ -18062,7 +18062,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B17">
         <v>256.10000000000002</v>
@@ -18071,7 +18071,7 @@
         <v>409</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H17">
         <v>307.62</v>
@@ -18080,7 +18080,7 @@
         <v>7</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="N17">
         <v>561.57000000000005</v>
@@ -18089,7 +18089,7 @@
         <v>7</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="T17">
         <v>175.27</v>
@@ -18100,7 +18100,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B18">
         <v>0.59</v>
@@ -18109,31 +18109,31 @@
         <v>153</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="H18">
         <v>0.24</v>
       </c>
       <c r="I18" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="S18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="T18">
         <v>0.88</v>
       </c>
       <c r="U18" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -18486,7 +18486,7 @@
         <v>-0.04</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="J26" s="21">
         <v>-0.28000000000000003</v>
@@ -18518,7 +18518,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="U26" s="28" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="V26" s="21">
         <v>1.37</v>
@@ -18554,7 +18554,7 @@
         <v>0.1</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="J27" s="16">
         <v>0.49</v>
@@ -18572,7 +18572,7 @@
         <v>0.02</v>
       </c>
       <c r="O27" s="27" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="P27" s="16">
         <v>7.0000000000000007E-2</v>
@@ -18590,7 +18590,7 @@
         <v>0.08</v>
       </c>
       <c r="U27" s="27" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="V27" s="16">
         <v>0.94</v>
@@ -18611,15 +18611,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0810E8FC-F61F-0644-9F5C-E92862BDCAF8}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>457</v>
+        <v>528</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -18645,7 +18645,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B5">
         <v>658.46</v>
@@ -18656,13 +18656,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B6">
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -18765,7 +18765,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D14" s="21">
         <v>-0.02</v>
@@ -18802,7 +18802,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B17">
         <v>361.16</v>
@@ -18813,13 +18813,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B18">
         <v>0.27</v>
       </c>
       <c r="C18" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -18922,7 +18922,7 @@
         <v>-0.06</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="D26" s="21">
         <v>-0.4</v>
@@ -18940,7 +18940,7 @@
         <v>0.13</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="D27" s="16">
         <v>0.52</v>

</xml_diff>